<commit_message>
Change data labels to reflect content
The generic _data.xmls content categories worked as a starting
point, but as the page templates are starting to get more complex,
it will be easier in the long run to make these labels more
semantically correct so that they are easier to recognize.

This commit also updates the classes.html page template variables
and renames categories.md to classes.md.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="460" windowWidth="29320" windowHeight="17760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27560" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
-    <sheet name="catalogue" sheetId="1" r:id="rId2"/>
+    <sheet name="classes" sheetId="1" r:id="rId2"/>
     <sheet name="directory" sheetId="3" r:id="rId3"/>
     <sheet name="feed" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">catalogue!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">classes!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">directory!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">feed!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$D$1</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="227">
   <si>
     <t>description</t>
   </si>
@@ -69,9 +69,6 @@
     <t>path</t>
   </si>
   <si>
-    <t>tags</t>
-  </si>
-  <si>
     <t>event-type</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>Catalogue</t>
-  </si>
-  <si>
     <t>Directory</t>
   </si>
   <si>
@@ -94,12 +88,6 @@
   </si>
   <si>
     <t>full-name</t>
-  </si>
-  <si>
-    <t>item-name</t>
-  </si>
-  <si>
-    <t>/catalogue.html</t>
   </si>
   <si>
     <t>/directory.html</t>
@@ -716,6 +704,15 @@
   </si>
   <si>
     <t>candy-hunt.png</t>
+  </si>
+  <si>
+    <t>class-name</t>
+  </si>
+  <si>
+    <t>/classes.html</t>
+  </si>
+  <si>
+    <t>Classes</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1349,7 +1346,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>10</v>
@@ -1357,10 +1354,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="9"/>
@@ -1369,28 +1366,28 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>226</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>23</v>
+        <v>225</v>
       </c>
       <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:6" s="23" customFormat="1">
       <c r="A4" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="24"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -1410,11 +1407,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1:X18"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1424,14 +1421,13 @@
     <col min="3" max="3" width="24" style="17" customWidth="1"/>
     <col min="4" max="5" width="12" style="17" customWidth="1"/>
     <col min="6" max="6" width="24" style="17" customWidth="1"/>
-    <col min="7" max="7" width="12" style="18" customWidth="1"/>
-    <col min="8" max="8" width="24" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="18"/>
+    <col min="7" max="7" width="24" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="21" customFormat="1">
+    <row r="1" spans="1:23" s="21" customFormat="1">
       <c r="A1" s="22" t="s">
-        <v>22</v>
+        <v>224</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -1440,108 +1436,105 @@
         <v>1</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="H1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="M1" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="N1" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="O1" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="P1" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="Q1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="R1" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="S1" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="T1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="U1" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="V1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="W1" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="35" t="s">
+    </row>
+    <row r="2" spans="1:23" ht="120">
+      <c r="A2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="I2" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="J2" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="120">
-      <c r="A2" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="36">
+      <c r="K2" s="36">
         <v>195</v>
       </c>
-      <c r="M2" s="30"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="36"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="30"/>
       <c r="Q2" s="30"/>
       <c r="R2" s="30"/>
       <c r="S2" s="30"/>
@@ -1549,47 +1542,46 @@
       <c r="U2" s="30"/>
       <c r="V2" s="30"/>
       <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-    </row>
-    <row r="3" spans="1:24" ht="128">
+    </row>
+    <row r="3" spans="1:23" ht="128">
       <c r="A3" s="25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="L3" s="36">
+      <c r="G3" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="36">
         <v>195</v>
       </c>
+      <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
       <c r="S3" s="30"/>
@@ -1597,43 +1589,42 @@
       <c r="U3" s="30"/>
       <c r="V3" s="30"/>
       <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-    </row>
-    <row r="4" spans="1:24" ht="135">
+    </row>
+    <row r="4" spans="1:23" ht="135">
       <c r="A4" s="25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="L4" s="36">
+      <c r="G4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="36">
         <v>196</v>
       </c>
+      <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
@@ -1645,299 +1636,294 @@
       <c r="U4" s="30"/>
       <c r="V4" s="30"/>
       <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-    </row>
-    <row r="5" spans="1:24" ht="330">
+    </row>
+    <row r="5" spans="1:23" ht="330">
       <c r="A5" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" s="30"/>
-      <c r="G5" s="17"/>
+      <c r="G5" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="H5" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="I5" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="K5" s="36">
+        <v>88</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="M5" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="N5" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="O5" s="36">
+        <v>88</v>
+      </c>
+      <c r="P5" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="Q5" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="R5" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="S5" s="38">
+        <v>88</v>
+      </c>
+      <c r="T5" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="L5" s="36">
+      <c r="U5" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="V5" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="W5" s="36">
         <v>88</v>
       </c>
-      <c r="M5" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="N5" s="30" t="s">
+    </row>
+    <row r="6" spans="1:23" ht="80">
+      <c r="A6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="O5" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="P5" s="36">
-        <v>88</v>
-      </c>
-      <c r="Q5" s="37" t="s">
+      <c r="I6" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="R5" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="S5" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="T5" s="38">
-        <v>88</v>
-      </c>
-      <c r="U5" s="30" t="s">
+      <c r="K6" s="36">
+        <v>60</v>
+      </c>
+      <c r="L6" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="W5" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="X5" s="36">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="80">
-      <c r="A6" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L6" s="36">
+      <c r="M6" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="N6" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="O6" s="36">
         <v>60</v>
       </c>
-      <c r="M6" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="O6" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="P6" s="36">
-        <v>60</v>
-      </c>
+      <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="30"/>
       <c r="U6" s="30"/>
       <c r="V6" s="30"/>
       <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-    </row>
-    <row r="7" spans="1:24" ht="60">
+    </row>
+    <row r="7" spans="1:23" ht="60">
       <c r="A7" s="25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="L7" s="36">
+      <c r="G7" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="K7" s="36">
         <v>55</v>
       </c>
-      <c r="M7" s="39" t="s">
-        <v>140</v>
+      <c r="L7" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="M7" s="30" t="s">
+        <v>117</v>
       </c>
       <c r="N7" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="O7" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="P7" s="36">
+        <v>135</v>
+      </c>
+      <c r="O7" s="36">
         <v>55</v>
       </c>
+      <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
       <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="30"/>
       <c r="U7" s="30"/>
       <c r="V7" s="30"/>
       <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-    </row>
-    <row r="8" spans="1:24" ht="60">
+    </row>
+    <row r="8" spans="1:23" ht="60">
       <c r="A8" s="25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="36">
+      <c r="G8" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8" s="36">
         <v>40</v>
       </c>
+      <c r="L8" s="30" t="s">
+        <v>139</v>
+      </c>
       <c r="M8" s="30" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="N8" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="O8" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="P8" s="36">
+        <v>138</v>
+      </c>
+      <c r="O8" s="36">
         <v>40</v>
       </c>
+      <c r="P8" s="30" t="s">
+        <v>140</v>
+      </c>
       <c r="Q8" s="30" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="R8" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="S8" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="T8" s="36">
+        <v>138</v>
+      </c>
+      <c r="S8" s="36">
         <v>50</v>
       </c>
+      <c r="T8" s="30"/>
       <c r="U8" s="30"/>
       <c r="V8" s="30"/>
       <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-    </row>
-    <row r="9" spans="1:24" ht="80">
+    </row>
+    <row r="9" spans="1:23" ht="80">
       <c r="A9" s="25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="30" t="s">
+      <c r="G9" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="36">
+        <v>80</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="M9" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="N9" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="J9" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="L9" s="36">
+      <c r="O9" s="36">
         <v>80</v>
       </c>
-      <c r="M9" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="O9" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="P9" s="36">
-        <v>80</v>
-      </c>
+      <c r="P9" s="30"/>
       <c r="Q9" s="30"/>
       <c r="R9" s="30"/>
       <c r="S9" s="30"/>
@@ -1945,52 +1931,52 @@
       <c r="U9" s="30"/>
       <c r="V9" s="30"/>
       <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-    </row>
-    <row r="10" spans="1:24" ht="135">
+    </row>
+    <row r="10" spans="1:23" ht="135">
       <c r="A10" s="25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F10" s="30"/>
-      <c r="H10" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="L10" s="36">
+      <c r="G10" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" s="36">
         <v>60</v>
       </c>
+      <c r="L10" s="30" t="s">
+        <v>148</v>
+      </c>
       <c r="M10" s="30" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="N10" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="O10" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="P10" s="36">
+        <v>147</v>
+      </c>
+      <c r="O10" s="36">
         <v>60</v>
       </c>
+      <c r="P10" s="30"/>
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="30"/>
@@ -1998,43 +1984,42 @@
       <c r="U10" s="30"/>
       <c r="V10" s="30"/>
       <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-    </row>
-    <row r="11" spans="1:24" ht="165">
+    </row>
+    <row r="11" spans="1:23" ht="165">
       <c r="A11" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C11" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="L11" s="36">
+      <c r="G11" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="36">
         <v>195</v>
       </c>
+      <c r="L11" s="30"/>
       <c r="M11" s="30"/>
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
@@ -2046,239 +2031,235 @@
       <c r="U11" s="30"/>
       <c r="V11" s="30"/>
       <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-    </row>
-    <row r="12" spans="1:24" ht="195">
+    </row>
+    <row r="12" spans="1:23" ht="195">
       <c r="A12" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="L12" s="36">
+      <c r="G12" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="K12" s="36">
         <v>55</v>
       </c>
+      <c r="L12" s="30" t="s">
+        <v>150</v>
+      </c>
       <c r="M12" s="30" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="N12" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="O12" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="P12" s="36">
+        <v>135</v>
+      </c>
+      <c r="O12" s="36">
         <v>55</v>
       </c>
+      <c r="P12" s="30"/>
       <c r="Q12" s="30"/>
       <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="30"/>
       <c r="U12" s="30"/>
       <c r="V12" s="30"/>
       <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-    </row>
-    <row r="13" spans="1:24" ht="165">
+    </row>
+    <row r="13" spans="1:23" ht="165">
       <c r="A13" s="25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="K13" s="36">
+        <v>12</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="M13" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="N13" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="O13" s="36">
+        <v>12</v>
+      </c>
+      <c r="P13" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="J13" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="L13" s="36">
-        <v>12</v>
-      </c>
-      <c r="M13" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="O13" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="P13" s="36">
-        <v>12</v>
-      </c>
-      <c r="Q13" s="32" t="s">
-        <v>159</v>
+      <c r="Q13" s="30" t="s">
+        <v>152</v>
       </c>
       <c r="R13" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="S13" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="T13" s="36">
+        <v>153</v>
+      </c>
+      <c r="S13" s="36">
         <v>16</v>
       </c>
+      <c r="T13" s="30"/>
       <c r="U13" s="30"/>
       <c r="V13" s="30"/>
       <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-    </row>
-    <row r="14" spans="1:24" ht="96">
+    </row>
+    <row r="14" spans="1:23" ht="96">
       <c r="A14" s="25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="36">
+        <v>12</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="N14" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" s="36">
+        <v>12</v>
+      </c>
+      <c r="P14" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="J14" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="L14" s="36">
-        <v>12</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="N14" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="O14" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="P14" s="36">
-        <v>12</v>
-      </c>
-      <c r="Q14" s="32" t="s">
-        <v>159</v>
+      <c r="Q14" s="30" t="s">
+        <v>152</v>
       </c>
       <c r="R14" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="S14" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="T14" s="36">
+        <v>153</v>
+      </c>
+      <c r="S14" s="36">
         <v>16</v>
       </c>
+      <c r="T14" s="30"/>
       <c r="U14" s="30"/>
       <c r="V14" s="30"/>
       <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-    </row>
-    <row r="15" spans="1:24" ht="120">
+    </row>
+    <row r="15" spans="1:23" ht="120">
       <c r="A15" s="25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="K15" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="L15" s="36">
+      <c r="G15" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="K15" s="36">
         <v>60</v>
       </c>
-      <c r="M15" s="32" t="s">
-        <v>162</v>
+      <c r="L15" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="O15" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="P15" s="36">
+        <v>157</v>
+      </c>
+      <c r="O15" s="36">
         <v>60</v>
       </c>
+      <c r="P15" s="30"/>
       <c r="Q15" s="30"/>
       <c r="R15" s="30"/>
       <c r="S15" s="30"/>
@@ -2286,165 +2267,164 @@
       <c r="U15" s="30"/>
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-    </row>
-    <row r="16" spans="1:24" ht="90">
+    </row>
+    <row r="16" spans="1:23" ht="90">
       <c r="A16" s="25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D16" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>75</v>
-      </c>
       <c r="F16" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="K16" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="L16" s="36">
+        <v>82</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="K16" s="36">
         <v>12</v>
       </c>
-      <c r="M16" s="40" t="s">
-        <v>130</v>
+      <c r="L16" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="M16" s="30" t="s">
+        <v>127</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="O16" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="P16" s="36">
+        <v>157</v>
+      </c>
+      <c r="O16" s="36">
         <v>12</v>
       </c>
+      <c r="P16" s="30" t="s">
+        <v>129</v>
+      </c>
       <c r="Q16" s="30" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="R16" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="S16" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="T16" s="36">
+        <v>157</v>
+      </c>
+      <c r="S16" s="36">
         <v>12</v>
       </c>
+      <c r="T16" s="30"/>
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
       <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-    </row>
-    <row r="17" spans="1:24" ht="180">
+    </row>
+    <row r="17" spans="1:23" ht="180">
       <c r="A17" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E17" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="K17" s="36">
         <v>75</v>
       </c>
-      <c r="F17" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="L17" s="36">
-        <v>75</v>
-      </c>
+      <c r="L17" s="30"/>
       <c r="M17" s="30"/>
       <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="37"/>
       <c r="Q17" s="37"/>
       <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="30"/>
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="36"/>
-    </row>
-    <row r="18" spans="1:24" s="17" customFormat="1" ht="160">
+      <c r="W17" s="36"/>
+    </row>
+    <row r="18" spans="1:23" s="17" customFormat="1" ht="160">
       <c r="A18" s="25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>99</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="K18" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="L18" s="36">
+        <v>156</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="36">
         <v>60</v>
       </c>
-      <c r="M18" s="32" t="s">
-        <v>162</v>
+      <c r="L18" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="O18" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="P18" s="36">
+        <v>157</v>
+      </c>
+      <c r="O18" s="36">
         <v>60</v>
       </c>
+      <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
@@ -2452,19 +2432,18 @@
       <c r="U18" s="25"/>
       <c r="V18" s="25"/>
       <c r="W18" s="25"/>
-      <c r="X18" s="25"/>
-    </row>
-    <row r="19" spans="1:24">
+    </row>
+    <row r="19" spans="1:23">
       <c r="B19" s="20"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:23">
       <c r="B20" s="20"/>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:23">
       <c r="B21" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H2"/>
+  <autoFilter ref="A1:G2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2500,7 +2479,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -2514,191 +2493,191 @@
     </row>
     <row r="2" spans="1:6" ht="90">
       <c r="A2" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C2" s="19" t="str">
         <f>A2&amp;" "&amp;B2</f>
         <v>Jocelyn Yee</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C3" s="19" t="str">
         <f t="shared" ref="C3:C10" si="0">A3&amp;" "&amp;B3</f>
         <v>Natalie Phillips</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="130">
       <c r="A4" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Brandon Murray</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105">
       <c r="A5" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Lydia Neal</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="150">
       <c r="A6" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Sarah Porter</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90">
       <c r="A7" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Avery Douglas</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90">
       <c r="A8" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Ramona Stephens</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="105">
       <c r="A9" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Javier Fletcher</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="65">
       <c r="A10" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C10" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Ana Andrews</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2783,7 +2762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -2807,22 +2786,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
@@ -2830,135 +2809,135 @@
     </row>
     <row r="2" spans="1:9" ht="75">
       <c r="A2" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>208</v>
-      </c>
       <c r="C2" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>219</v>
-      </c>
       <c r="H2" s="46" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>209</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>210</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60">
       <c r="A5" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B5" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="E5" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60">
       <c r="A6" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B6" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:9">

</xml_diff>

<commit_message>
Create category navigation taxonomy & page
Create category navigation taxonomy in data file to generate pages
for individual class categories. Update category.html to show class
category groupings and add “all programs” category nav to
navigate between categories.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27560" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="740" windowWidth="23920" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
-    <sheet name="classes" sheetId="1" r:id="rId2"/>
-    <sheet name="directory" sheetId="3" r:id="rId3"/>
-    <sheet name="feed" sheetId="2" r:id="rId4"/>
+    <sheet name="categories" sheetId="5" r:id="rId2"/>
+    <sheet name="classes" sheetId="1" r:id="rId3"/>
+    <sheet name="directory" sheetId="3" r:id="rId4"/>
+    <sheet name="feed" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">classes!$A$1:$G$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">directory!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">feed!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">classes!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">directory!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">feed!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="236">
   <si>
     <t>description</t>
   </si>
@@ -88,6 +90,9 @@
   </si>
   <si>
     <t>full-name</t>
+  </si>
+  <si>
+    <t>/catalogue.html</t>
   </si>
   <si>
     <t>/directory.html</t>
@@ -709,10 +714,34 @@
     <t>class-name</t>
   </si>
   <si>
-    <t>/classes.html</t>
-  </si>
-  <si>
     <t>Classes</t>
+  </si>
+  <si>
+    <t>category-label</t>
+  </si>
+  <si>
+    <t>Visual Arts &amp; Crafts</t>
+  </si>
+  <si>
+    <t>arts-crafts.png</t>
+  </si>
+  <si>
+    <t>Fitness, Health &amp; Wellness</t>
+  </si>
+  <si>
+    <t>fitness.png</t>
+  </si>
+  <si>
+    <t>Performing Arts &amp; Dance</t>
+  </si>
+  <si>
+    <t>performing-arts.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athletics </t>
+  </si>
+  <si>
+    <t>athletics.png</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1356,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1369,7 +1398,7 @@
         <v>226</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>225</v>
+        <v>20</v>
       </c>
       <c r="C3" s="16"/>
     </row>
@@ -1378,7 +1407,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="24"/>
     </row>
@@ -1387,7 +1416,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -1406,6 +1435,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W21"/>
   <sheetViews>
@@ -1427,7 +1540,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="21" customFormat="1">
       <c r="A1" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -1436,96 +1549,96 @@
         <v>1</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P1" s="33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q1" s="33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S1" s="33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="120">
       <c r="A2" s="25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K2" s="36">
         <v>195</v>
@@ -1545,34 +1658,34 @@
     </row>
     <row r="3" spans="1:23" ht="128">
       <c r="A3" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K3" s="36">
         <v>195</v>
@@ -1592,34 +1705,34 @@
     </row>
     <row r="4" spans="1:23" ht="135">
       <c r="A4" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H4" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="30" t="s">
         <v>121</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>120</v>
       </c>
       <c r="K4" s="36">
         <v>196</v>
@@ -1639,68 +1752,68 @@
     </row>
     <row r="5" spans="1:23" ht="330">
       <c r="A5" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K5" s="36">
         <v>88</v>
       </c>
       <c r="L5" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="M5" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>125</v>
       </c>
       <c r="O5" s="36">
         <v>88</v>
       </c>
       <c r="P5" s="37" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R5" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="S5" s="38">
         <v>88</v>
       </c>
       <c r="T5" s="30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="U5" s="30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="V5" s="30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="W5" s="36">
         <v>88</v>
@@ -1708,44 +1821,44 @@
     </row>
     <row r="6" spans="1:23" ht="80">
       <c r="A6" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" s="36">
         <v>60</v>
       </c>
       <c r="L6" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="30" t="s">
         <v>133</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>132</v>
       </c>
       <c r="O6" s="36">
         <v>60</v>
@@ -1761,46 +1874,46 @@
     </row>
     <row r="7" spans="1:23" ht="60">
       <c r="A7" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K7" s="36">
         <v>55</v>
       </c>
       <c r="L7" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="M7" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="30" t="s">
         <v>136</v>
-      </c>
-      <c r="M7" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>135</v>
       </c>
       <c r="O7" s="36">
         <v>55</v>
@@ -1816,58 +1929,58 @@
     </row>
     <row r="8" spans="1:23" ht="60">
       <c r="A8" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K8" s="36">
         <v>40</v>
       </c>
       <c r="L8" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" s="30" t="s">
         <v>139</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="N8" s="30" t="s">
-        <v>138</v>
       </c>
       <c r="O8" s="36">
         <v>40</v>
       </c>
       <c r="P8" s="30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="Q8" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R8" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S8" s="36">
         <v>50</v>
@@ -1879,46 +1992,46 @@
     </row>
     <row r="9" spans="1:23" ht="80">
       <c r="A9" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K9" s="36">
         <v>80</v>
       </c>
       <c r="L9" s="30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N9" s="30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O9" s="36">
         <v>80</v>
@@ -1934,44 +2047,44 @@
     </row>
     <row r="10" spans="1:23" ht="135">
       <c r="A10" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K10" s="36">
         <v>60</v>
       </c>
       <c r="L10" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="M10" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" s="30" t="s">
         <v>148</v>
-      </c>
-      <c r="M10" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="N10" s="30" t="s">
-        <v>147</v>
       </c>
       <c r="O10" s="36">
         <v>60</v>
@@ -1987,34 +2100,34 @@
     </row>
     <row r="11" spans="1:23" ht="165">
       <c r="A11" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>72</v>
-      </c>
       <c r="F11" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H11" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="30" t="s">
         <v>119</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="K11" s="36">
         <v>195</v>
@@ -2034,46 +2147,46 @@
     </row>
     <row r="12" spans="1:23" ht="195">
       <c r="A12" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K12" s="36">
         <v>55</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M12" s="30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N12" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O12" s="36">
         <v>55</v>
@@ -2089,58 +2202,58 @@
     </row>
     <row r="13" spans="1:23" ht="165">
       <c r="A13" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K13" s="36">
         <v>12</v>
       </c>
       <c r="L13" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="N13" s="30" t="s">
         <v>154</v>
-      </c>
-      <c r="M13" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>153</v>
       </c>
       <c r="O13" s="36">
         <v>12</v>
       </c>
       <c r="P13" s="32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q13" s="30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R13" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="S13" s="36">
         <v>16</v>
@@ -2152,58 +2265,58 @@
     </row>
     <row r="14" spans="1:23" ht="96">
       <c r="A14" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K14" s="36">
         <v>12</v>
       </c>
       <c r="L14" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="N14" s="30" t="s">
         <v>154</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="N14" s="30" t="s">
-        <v>153</v>
       </c>
       <c r="O14" s="36">
         <v>12</v>
       </c>
       <c r="P14" s="32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q14" s="30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R14" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="S14" s="36">
         <v>16</v>
@@ -2215,46 +2328,46 @@
     </row>
     <row r="15" spans="1:23" ht="120">
       <c r="A15" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K15" s="36">
         <v>60</v>
       </c>
       <c r="L15" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="M15" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N15" s="30" t="s">
         <v>158</v>
-      </c>
-      <c r="M15" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="N15" s="30" t="s">
-        <v>157</v>
       </c>
       <c r="O15" s="36">
         <v>60</v>
@@ -2270,58 +2383,58 @@
     </row>
     <row r="16" spans="1:23" ht="90">
       <c r="A16" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K16" s="36">
         <v>12</v>
       </c>
       <c r="L16" s="40" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O16" s="36">
         <v>12</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q16" s="30" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R16" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="S16" s="36">
         <v>12</v>
@@ -2333,34 +2446,34 @@
     </row>
     <row r="17" spans="1:23" ht="180">
       <c r="A17" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K17" s="36">
         <v>75</v>
@@ -2380,46 +2493,46 @@
     </row>
     <row r="18" spans="1:23" s="17" customFormat="1" ht="160">
       <c r="A18" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J18" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K18" s="36">
         <v>60</v>
       </c>
       <c r="L18" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N18" s="30" t="s">
         <v>158</v>
-      </c>
-      <c r="M18" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="N18" s="30" t="s">
-        <v>157</v>
       </c>
       <c r="O18" s="36">
         <v>60</v>
@@ -2454,7 +2567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -2493,191 +2606,191 @@
     </row>
     <row r="2" spans="1:6" ht="90">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C2" s="19" t="str">
         <f>A2&amp;" "&amp;B2</f>
         <v>Jocelyn Yee</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120">
       <c r="A3" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C3" s="19" t="str">
         <f t="shared" ref="C3:C10" si="0">A3&amp;" "&amp;B3</f>
         <v>Natalie Phillips</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="130">
       <c r="A4" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Brandon Murray</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Lydia Neal</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="150">
       <c r="A6" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Sarah Porter</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90">
       <c r="A7" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Avery Douglas</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90">
       <c r="A8" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Ramona Stephens</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="105">
       <c r="A9" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Javier Fletcher</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="65">
       <c r="A10" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C10" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Ana Andrews</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2758,7 +2871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
@@ -2792,16 +2905,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
@@ -2809,135 +2922,135 @@
     </row>
     <row r="2" spans="1:9" ht="75">
       <c r="A2" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H2" s="46" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>216</v>
-      </c>
       <c r="I3" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60">
       <c r="A5" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60">
       <c r="A6" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:9">

</xml_diff>

<commit_message>
Create global nav drawer
Update Navigation sheet of _data file to reflect a category
structure in the drawer nav. Responsive drawer nav pattern is
moved from an include to the default page for clarity – there
is a whole-page wrap that occurs that is hard to follow if
opening and closing divs appear in different includes.

This commit also removes CSS that applies only to the original
nav-bar pattern as well as the original nav-bar include.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="740" windowWidth="23920" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19840" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="235">
   <si>
     <t>description</t>
   </si>
@@ -83,22 +83,7 @@
     <t>/</t>
   </si>
   <si>
-    <t>Directory</t>
-  </si>
-  <si>
-    <t>Events</t>
-  </si>
-  <si>
     <t>full-name</t>
-  </si>
-  <si>
-    <t>/catalogue.html</t>
-  </si>
-  <si>
-    <t>/directory.html</t>
-  </si>
-  <si>
-    <t>/events.html</t>
   </si>
   <si>
     <t>age</t>
@@ -714,9 +699,6 @@
     <t>class-name</t>
   </si>
   <si>
-    <t>Classes</t>
-  </si>
-  <si>
     <t>category-label</t>
   </si>
   <si>
@@ -742,6 +724,21 @@
   </si>
   <si>
     <t>athletics.png</t>
+  </si>
+  <si>
+    <t>Center Programs</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Contact Information</t>
+  </si>
+  <si>
+    <t>Seattle Parks &amp; Recreation</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -892,7 +889,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -959,7 +956,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1353,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1395,33 +1391,32 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" s="23" customFormat="1">
-      <c r="A4" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="24"/>
+        <v>230</v>
+      </c>
+      <c r="B3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>22</v>
+        <v>233</v>
+      </c>
+      <c r="B5" t="s">
+        <v>231</v>
       </c>
       <c r="C5" s="16"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
@@ -1454,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>11</v>
@@ -1462,48 +1457,48 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1540,7 +1535,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="21" customFormat="1">
       <c r="A1" s="22" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -1549,1002 +1544,1002 @@
         <v>1</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="N1" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="O1" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="P1" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="Q1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="R1" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="S1" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="T1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="U1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="V1" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="W1" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="33" t="s">
+    </row>
+    <row r="2" spans="1:23" ht="120">
+      <c r="A2" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="I2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="J2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="K2" s="35">
+        <v>195</v>
+      </c>
+      <c r="L2" s="29"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+    </row>
+    <row r="3" spans="1:23" ht="128">
+      <c r="A3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="I3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J3" s="29" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="120">
-      <c r="A2" s="25" t="s">
+      <c r="K3" s="35">
+        <v>195</v>
+      </c>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+    </row>
+    <row r="4" spans="1:23" ht="135">
+      <c r="A4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="35">
+        <v>196</v>
+      </c>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+    </row>
+    <row r="5" spans="1:23" ht="330">
+      <c r="A5" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="35">
+        <v>88</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="N5" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="O5" s="35">
+        <v>88</v>
+      </c>
+      <c r="P5" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q5" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="R5" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="S5" s="37">
+        <v>88</v>
+      </c>
+      <c r="T5" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="U5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="V5" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="W5" s="35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="80">
+      <c r="A6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" s="35">
+        <v>60</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="O6" s="35">
+        <v>60</v>
+      </c>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+    </row>
+    <row r="7" spans="1:23" ht="60">
+      <c r="A7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="G7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="K7" s="35">
+        <v>55</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="O7" s="35">
+        <v>55</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+    </row>
+    <row r="8" spans="1:23" ht="60">
+      <c r="A8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="35">
+        <v>40</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="O8" s="35">
+        <v>40</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="R8" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="S8" s="35">
+        <v>50</v>
+      </c>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+    </row>
+    <row r="9" spans="1:23" ht="80">
+      <c r="A9" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="35">
+        <v>80</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="O9" s="35">
+        <v>80</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+    </row>
+    <row r="10" spans="1:23" ht="135">
+      <c r="A10" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="K10" s="35">
         <v>60</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="L10" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="N10" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="O10" s="35">
+        <v>60</v>
+      </c>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+    </row>
+    <row r="11" spans="1:23" ht="165">
+      <c r="A11" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="35">
+        <v>195</v>
+      </c>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+    </row>
+    <row r="12" spans="1:23" ht="195">
+      <c r="A12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="D12" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" s="35">
+        <v>55</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="O12" s="35">
+        <v>55</v>
+      </c>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+    </row>
+    <row r="13" spans="1:23" ht="165">
+      <c r="A13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="K13" s="35">
+        <v>12</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="N13" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="O13" s="35">
+        <v>12</v>
+      </c>
+      <c r="P13" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q13" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="R13" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="S13" s="35">
+        <v>16</v>
+      </c>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+    </row>
+    <row r="14" spans="1:23" ht="96">
+      <c r="A14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="K14" s="35">
+        <v>12</v>
+      </c>
+      <c r="L14" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="O14" s="35">
+        <v>12</v>
+      </c>
+      <c r="P14" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q14" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="R14" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="S14" s="35">
+        <v>16</v>
+      </c>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+    </row>
+    <row r="15" spans="1:23" ht="120">
+      <c r="A15" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="K15" s="35">
+        <v>60</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="O15" s="35">
+        <v>60</v>
+      </c>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+    </row>
+    <row r="16" spans="1:23" ht="90">
+      <c r="A16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" s="25" t="s">
+      <c r="G16" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="K16" s="35">
+        <v>12</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="N16" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="O16" s="35">
+        <v>12</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="R16" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="S16" s="35">
+        <v>12</v>
+      </c>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+    </row>
+    <row r="17" spans="1:23" ht="180">
+      <c r="A17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" s="35">
+        <v>75</v>
+      </c>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="35"/>
+    </row>
+    <row r="18" spans="1:23" s="17" customFormat="1" ht="160">
+      <c r="A18" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="I18" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2" s="36">
-        <v>195</v>
-      </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-    </row>
-    <row r="3" spans="1:23" ht="128">
-      <c r="A3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="29" t="s">
+      <c r="J18" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="K18" s="35">
         <v>60</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="25" t="s">
+      <c r="L18" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="M18" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="K3" s="36">
-        <v>195</v>
-      </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-    </row>
-    <row r="4" spans="1:23" ht="135">
-      <c r="A4" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="29" t="s">
+      <c r="N18" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="O18" s="35">
         <v>60</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="K4" s="36">
-        <v>196</v>
-      </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-    </row>
-    <row r="5" spans="1:23" ht="330">
-      <c r="A5" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="K5" s="36">
-        <v>88</v>
-      </c>
-      <c r="L5" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="M5" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="O5" s="36">
-        <v>88</v>
-      </c>
-      <c r="P5" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q5" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="R5" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="S5" s="38">
-        <v>88</v>
-      </c>
-      <c r="T5" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="U5" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="V5" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="W5" s="36">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="80">
-      <c r="A6" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="K6" s="36">
-        <v>60</v>
-      </c>
-      <c r="L6" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="O6" s="36">
-        <v>60</v>
-      </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-    </row>
-    <row r="7" spans="1:23" ht="60">
-      <c r="A7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="K7" s="36">
-        <v>55</v>
-      </c>
-      <c r="L7" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="M7" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="O7" s="36">
-        <v>55</v>
-      </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-    </row>
-    <row r="8" spans="1:23" ht="60">
-      <c r="A8" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="K8" s="36">
-        <v>40</v>
-      </c>
-      <c r="L8" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="N8" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="O8" s="36">
-        <v>40</v>
-      </c>
-      <c r="P8" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q8" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="R8" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="S8" s="36">
-        <v>50</v>
-      </c>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="30"/>
-    </row>
-    <row r="9" spans="1:23" ht="80">
-      <c r="A9" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="K9" s="36">
-        <v>80</v>
-      </c>
-      <c r="L9" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="M9" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="O9" s="36">
-        <v>80</v>
-      </c>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-    </row>
-    <row r="10" spans="1:23" ht="135">
-      <c r="A10" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="K10" s="36">
-        <v>60</v>
-      </c>
-      <c r="L10" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="M10" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="N10" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="O10" s="36">
-        <v>60</v>
-      </c>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-    </row>
-    <row r="11" spans="1:23" ht="165">
-      <c r="A11" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="K11" s="36">
-        <v>195</v>
-      </c>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-    </row>
-    <row r="12" spans="1:23" ht="195">
-      <c r="A12" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="K12" s="36">
-        <v>55</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="M12" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="N12" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="O12" s="36">
-        <v>55</v>
-      </c>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-    </row>
-    <row r="13" spans="1:23" ht="165">
-      <c r="A13" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="J13" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="K13" s="36">
-        <v>12</v>
-      </c>
-      <c r="L13" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="M13" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="O13" s="36">
-        <v>12</v>
-      </c>
-      <c r="P13" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q13" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="R13" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="S13" s="36">
-        <v>16</v>
-      </c>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-    </row>
-    <row r="14" spans="1:23" ht="96">
-      <c r="A14" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="K14" s="36">
-        <v>12</v>
-      </c>
-      <c r="L14" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="N14" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="O14" s="36">
-        <v>12</v>
-      </c>
-      <c r="P14" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q14" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="R14" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="S14" s="36">
-        <v>16</v>
-      </c>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-    </row>
-    <row r="15" spans="1:23" ht="120">
-      <c r="A15" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="J15" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="K15" s="36">
-        <v>60</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="M15" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="N15" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="O15" s="36">
-        <v>60</v>
-      </c>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
-    </row>
-    <row r="16" spans="1:23" ht="90">
-      <c r="A16" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J16" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="K16" s="36">
-        <v>12</v>
-      </c>
-      <c r="L16" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="M16" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="N16" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="O16" s="36">
-        <v>12</v>
-      </c>
-      <c r="P16" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q16" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="R16" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="S16" s="36">
-        <v>12</v>
-      </c>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-    </row>
-    <row r="17" spans="1:23" ht="180">
-      <c r="A17" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="K17" s="36">
-        <v>75</v>
-      </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="36"/>
-    </row>
-    <row r="18" spans="1:23" s="17" customFormat="1" ht="160">
-      <c r="A18" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="K18" s="36">
-        <v>60</v>
-      </c>
-      <c r="L18" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="M18" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="N18" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="O18" s="36">
-        <v>60</v>
-      </c>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
-      <c r="U18" s="25"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="25"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
     </row>
     <row r="19" spans="1:23">
       <c r="B19" s="20"/>
@@ -2572,7 +2567,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2592,7 +2587,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -2606,191 +2601,191 @@
     </row>
     <row r="2" spans="1:6" ht="90">
       <c r="A2" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C2" s="19" t="str">
         <f>A2&amp;" "&amp;B2</f>
         <v>Jocelyn Yee</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120">
       <c r="A3" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C3" s="19" t="str">
         <f t="shared" ref="C3:C10" si="0">A3&amp;" "&amp;B3</f>
         <v>Natalie Phillips</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="130">
       <c r="A4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Brandon Murray</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105">
       <c r="A5" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Lydia Neal</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="150">
       <c r="A6" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Sarah Porter</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E6" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90">
       <c r="A7" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Avery Douglas</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90">
       <c r="A8" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Ramona Stephens</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="105">
       <c r="A9" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Javier Fletcher</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="65">
       <c r="A10" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C10" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Ana Andrews</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2905,16 +2900,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>215</v>
+        <v>18</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>210</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
@@ -2922,135 +2917,135 @@
     </row>
     <row r="2" spans="1:9" ht="75">
       <c r="A2" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>205</v>
+        <v>196</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>200</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="45" t="s">
         <v>212</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>206</v>
+        <v>197</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>201</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>209</v>
+        <v>67</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>204</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60">
       <c r="A5" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60">
       <c r="A6" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:9">

</xml_diff>

<commit_message>
Create home page events block
This commit includes changing th name of Feeds sheet to
Events for clarity.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19840" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="16040" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
     <sheet name="categories" sheetId="5" r:id="rId2"/>
     <sheet name="classes" sheetId="1" r:id="rId3"/>
     <sheet name="directory" sheetId="3" r:id="rId4"/>
-    <sheet name="feed" sheetId="2" r:id="rId5"/>
+    <sheet name="events" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">classes!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">directory!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">feed!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">events!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -638,9 +638,6 @@
     <t>2016-01-16</t>
   </si>
   <si>
-    <t>2016-03-25</t>
-  </si>
-  <si>
     <t>ongoing</t>
   </si>
   <si>
@@ -669,9 +666,6 @@
     <t>cost</t>
   </si>
   <si>
-    <t>12-4:00 pm</t>
-  </si>
-  <si>
     <t>free</t>
   </si>
   <si>
@@ -739,6 +733,12 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>2017-03-25</t>
+  </si>
+  <si>
+    <t>12-4 pm</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -1391,30 +1391,30 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -1449,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>11</v>
@@ -1460,10 +1460,10 @@
         <v>69</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
@@ -1473,10 +1473,10 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1484,10 +1484,10 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1495,10 +1495,10 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1535,7 +1535,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="21" customFormat="1">
       <c r="A1" s="22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -2870,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2903,13 +2903,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="H1" s="44" t="s">
         <v>209</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>210</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
@@ -2926,19 +2926,19 @@
         <v>67</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>126</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="H2" s="45" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2946,28 +2946,28 @@
         <v>197</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
@@ -2975,25 +2975,25 @@
         <v>198</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>149</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60">
@@ -3001,25 +3001,25 @@
         <v>199</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>207</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60">
@@ -3027,25 +3027,25 @@
         <v>199</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>207</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>126</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9">

</xml_diff>

<commit_message>
Add age-group focused program nav
Add “supplemental” age group based categories to “categories”
data sheet. Create age group based nav block on home screen.
Add filtered class tile view to age group based screens.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="16040" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="16040" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="events" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$D$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">classes!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">directory!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">events!$A$1:$D$1</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="246">
   <si>
     <t>description</t>
   </si>
@@ -696,12 +696,18 @@
     <t>category-label</t>
   </si>
   <si>
+    <t>class</t>
+  </si>
+  <si>
     <t>Visual Arts &amp; Crafts</t>
   </si>
   <si>
     <t>arts-crafts.png</t>
   </si>
   <si>
+    <t>main</t>
+  </si>
+  <si>
     <t>Fitness, Health &amp; Wellness</t>
   </si>
   <si>
@@ -720,10 +726,37 @@
     <t>athletics.png</t>
   </si>
   <si>
+    <t>teens</t>
+  </si>
+  <si>
+    <t>Teen Programs</t>
+  </si>
+  <si>
+    <t>teen.png</t>
+  </si>
+  <si>
+    <t>supplemental</t>
+  </si>
+  <si>
+    <t>Tots Programs</t>
+  </si>
+  <si>
+    <t>tot.png</t>
+  </si>
+  <si>
+    <t>Senior Programs</t>
+  </si>
+  <si>
+    <t>senior.png</t>
+  </si>
+  <si>
     <t>Center Programs</t>
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>/categories/teens.html</t>
   </si>
   <si>
     <t>Contact Information</t>
@@ -1349,7 +1382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
@@ -1391,32 +1424,41 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
@@ -1431,17 +1473,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="1" max="2" width="36" customWidth="1"/>
+    <col min="3" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1454,18 +1495,23 @@
       <c r="C1" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="D1" s="11" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D2" s="7"/>
+        <v>222</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>223</v>
+      </c>
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5">
@@ -1473,9 +1519,12 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>223</v>
       </c>
     </row>
@@ -1484,10 +1533,13 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>227</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1495,14 +1547,59 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>229</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <autoFilter ref="A1:D8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1517,9 +1614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2335,7 +2432,7 @@
         <v>62</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>67</v>
+        <v>230</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>73</v>
@@ -2390,7 +2487,7 @@
         <v>63</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>67</v>
+        <v>230</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>78</v>
@@ -2500,7 +2597,7 @@
         <v>57</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>80</v>
@@ -2870,7 +2967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2935,7 +3032,7 @@
         <v>126</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="H2" s="45" t="s">
         <v>210</v>
@@ -2946,7 +3043,7 @@
         <v>197</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Create "more classes in this age group" nav
This commit repurposes the filtered class tile view used for age
based groups to create “more classes” lists on class detail pages
based on age groupings. The class-tile block is broken out into
its own include in order to reduce duplication and simplify code
across age and activity-type categories.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -1615,8 +1615,8 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>